<commit_message>
final update before branching for LUI
</commit_message>
<xml_diff>
--- a/lab2/Lab2 Test Analyses.xlsx
+++ b/lab2/Lab2 Test Analyses.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ostatemailokstate-my.sharepoint.com/personal/jarett_woodard_okstate_edu/Documents/Current Classes/Computer Architecture/Labs/ecen4243S25/lab2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="8_{9738267B-587C-4ACE-951C-B2C5EE3FB578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACF49EFD-A395-4B3D-BE32-B6566A441C59}"/>
+  <xr:revisionPtr revIDLastSave="233" documentId="8_{9738267B-587C-4ACE-951C-B2C5EE3FB578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8B393C7-C40A-4FBF-9D9A-2A5D47C67A14}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{0B9D6FCE-2961-4AEC-91F3-19D465256351}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{0B9D6FCE-2961-4AEC-91F3-19D465256351}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="xor" sheetId="2" r:id="rId2"/>
     <sheet name="xori" sheetId="3" r:id="rId3"/>
+    <sheet name="lui" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="78">
   <si>
     <t>1111 1111 1111 1111 1111 1111 1111 1111</t>
   </si>
@@ -1557,6 +1558,21 @@
   </si>
   <si>
     <t>FFFF FFFA</t>
+  </si>
+  <si>
+    <t>Modules to check</t>
+  </si>
+  <si>
+    <t>maindec</t>
+  </si>
+  <si>
+    <t>aludec</t>
+  </si>
+  <si>
+    <t>Main decoder</t>
+  </si>
+  <si>
+    <t>ALU decoder</t>
   </si>
 </sst>
 </file>
@@ -1670,14 +1686,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1753,8 +1769,8 @@
       <xdr:row>55</xdr:row>
       <xdr:rowOff>38154</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="8" name="Ink 7">
@@ -1773,7 +1789,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="8" name="Ink 7">
@@ -1818,8 +1834,8 @@
       <xdr:row>55</xdr:row>
       <xdr:rowOff>55794</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="15" name="Ink 14">
@@ -1838,7 +1854,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="15" name="Ink 14">
@@ -1883,8 +1899,8 @@
       <xdr:row>55</xdr:row>
       <xdr:rowOff>48594</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="17" name="Ink 16">
@@ -1903,7 +1919,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="17" name="Ink 16">
@@ -1948,8 +1964,8 @@
       <xdr:row>49</xdr:row>
       <xdr:rowOff>31375</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="21" name="Ink 20">
@@ -1968,7 +1984,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="21" name="Ink 20">
@@ -2013,8 +2029,8 @@
       <xdr:row>53</xdr:row>
       <xdr:rowOff>177614</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="24" name="Ink 23">
@@ -2033,7 +2049,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="24" name="Ink 23">
@@ -2923,8 +2939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33EA99D-DA8E-4C5D-A5CD-D0C7B6762F0F}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D39" zoomScale="124" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView topLeftCell="C30" zoomScale="124" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48:R56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2943,88 +2959,88 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -3058,7 +3074,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -3154,7 +3170,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3253,7 +3269,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -3352,7 +3368,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -3407,7 +3423,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -3483,7 +3499,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -3528,7 +3544,7 @@
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -3576,7 +3592,7 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -3607,7 +3623,7 @@
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -3653,17 +3669,17 @@
       <c r="E48" s="1">
         <v>6</v>
       </c>
-      <c r="M48" s="9"/>
-      <c r="N48" s="9">
+      <c r="M48" s="8"/>
+      <c r="N48" s="8">
         <v>3</v>
       </c>
-      <c r="O48" s="9">
+      <c r="O48" s="8">
         <v>2</v>
       </c>
-      <c r="P48" s="9">
+      <c r="P48" s="8">
         <v>1</v>
       </c>
-      <c r="Q48" s="9">
+      <c r="Q48" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3680,13 +3696,13 @@
       <c r="E49" s="1">
         <v>-1</v>
       </c>
-      <c r="M49" s="9">
+      <c r="M49" s="8">
         <v>31</v>
       </c>
-      <c r="N49" s="9"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="9"/>
-      <c r="Q49" s="9" t="s">
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3703,13 +3719,13 @@
       <c r="E50" s="1">
         <v>9</v>
       </c>
-      <c r="M50" s="9">
+      <c r="M50" s="8">
         <v>27</v>
       </c>
-      <c r="N50" s="9"/>
-      <c r="O50" s="9"/>
-      <c r="P50" s="9"/>
-      <c r="Q50" s="9"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="8"/>
     </row>
     <row r="51" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
@@ -3724,13 +3740,13 @@
       <c r="E51" s="1">
         <v>6</v>
       </c>
-      <c r="M51" s="9">
+      <c r="M51" s="8">
         <v>23</v>
       </c>
-      <c r="N51" s="9"/>
-      <c r="O51" s="9"/>
-      <c r="P51" s="9"/>
-      <c r="Q51" s="9"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="8"/>
     </row>
     <row r="52" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
@@ -3745,57 +3761,699 @@
       <c r="E52" s="1">
         <v>0</v>
       </c>
-      <c r="M52" s="9">
+      <c r="M52" s="8">
         <v>19</v>
       </c>
-      <c r="N52" s="9"/>
-      <c r="O52" s="9"/>
-      <c r="P52" s="9"/>
-      <c r="Q52" s="9"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8"/>
     </row>
     <row r="53" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M53" s="9">
+      <c r="M53" s="8">
         <v>15</v>
       </c>
-      <c r="N53" s="9"/>
-      <c r="O53" s="9"/>
-      <c r="P53" s="9"/>
-      <c r="Q53" s="9"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M54" s="9">
+      <c r="M54" s="8">
         <v>11</v>
       </c>
-      <c r="N54" s="9"/>
-      <c r="O54" s="9" t="s">
+      <c r="N54" s="8"/>
+      <c r="O54" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="P54" s="9"/>
-      <c r="Q54" s="9"/>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="8"/>
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M55" s="9">
+      <c r="M55" s="8">
         <v>7</v>
       </c>
-      <c r="N55" s="9" t="s">
+      <c r="N55" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O55" s="9" t="s">
+      <c r="O55" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="P55" s="9" t="s">
+      <c r="P55" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q55" s="9"/>
+      <c r="Q55" s="8"/>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M56" s="9">
+      <c r="M56" s="8">
         <v>3</v>
       </c>
-      <c r="N56" s="9"/>
-      <c r="O56" s="9"/>
-      <c r="P56" s="9"/>
-      <c r="Q56" s="9"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2BF792-553E-4FD6-882B-DC81484ECAC2}">
+  <dimension ref="A1:Q56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="5"/>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="J2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="J3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16">
+        <v>-1</v>
+      </c>
+      <c r="J16" t="str">
+        <f>DEC2BIN(I16,8)</f>
+        <v>1111111111</v>
+      </c>
+      <c r="K16" t="str">
+        <f>BIN2HEX(J16)</f>
+        <v>FFFFFFFFFF</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="I17">
+        <v>-2</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" ref="J17:J33" si="0">DEC2BIN(I17,8)</f>
+        <v>1111111110</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" ref="K17:K33" si="1">BIN2HEX(J17)</f>
+        <v>FFFFFFFFFE</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="I18">
+        <v>-3</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>1111111101</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFFD</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="I19">
+        <v>-4</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>1111111100</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFFC</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="I20">
+        <f>I19-1</f>
+        <v>-5</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>1111111011</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFFB</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="I21">
+        <f t="shared" ref="I21:I33" si="2">I20-1</f>
+        <v>-6</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>1111111010</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFFA</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>-7</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="0"/>
+        <v>1111111001</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFF9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="0"/>
+        <v>1111111000</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFF8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="0"/>
+        <v>1111110111</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFF7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="0"/>
+        <v>1111110110</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFF6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>-11</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v>1111110101</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFF5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="I27">
+        <f>I26-1</f>
+        <v>-12</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="0"/>
+        <v>1111110100</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFF4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>-13</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="0"/>
+        <v>1111110011</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFF3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>-14</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="0"/>
+        <v>1111110010</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFF2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>-15</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="0"/>
+        <v>1111110001</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFF1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>-16</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="0"/>
+        <v>1111110000</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFF0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>-17</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="0"/>
+        <v>1111101111</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFEF</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>-18</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="0"/>
+        <v>1111101110</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFFEE</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8">
+        <v>3</v>
+      </c>
+      <c r="O48" s="8">
+        <v>2</v>
+      </c>
+      <c r="P48" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="M49" s="8">
+        <v>31</v>
+      </c>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="M50" s="8">
+        <v>27</v>
+      </c>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="8"/>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="M51" s="8">
+        <v>23</v>
+      </c>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="8"/>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="M52" s="8">
+        <v>19</v>
+      </c>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8"/>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M53" s="8">
+        <v>15</v>
+      </c>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="8"/>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M54" s="8">
+        <v>11</v>
+      </c>
+      <c r="N54" s="8"/>
+      <c r="O54" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="8"/>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M55" s="8">
+        <v>7</v>
+      </c>
+      <c r="N55" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O55" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P55" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q55" s="8"/>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M56" s="8">
+        <v>3</v>
+      </c>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3812,6 +4470,5 @@
     <mergeCell ref="A7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>